<commit_message>
Updating the testcases of converting module
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 2/Final-Project-Test-Cases-version-2.xlsx
+++ b/Documents/Test cases/Version 2/Final-Project-Test-Cases-version-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d68bcfb44c4b5b/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF874DA4-EB71-456F-BB22-38982AF81513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680095C8-FF14-4B8A-B372-8E9F7D77326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="104">
   <si>
     <t>Comments</t>
   </si>
@@ -1148,6 +1148,36 @@
   </si>
   <si>
     <t>The return length is correct.</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Testing the edge cases</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Testing if a long number works</t>
+  </si>
+  <si>
+    <t>"112233445566778899.000000"</t>
+  </si>
+  <si>
+    <t>"112233445566778899"</t>
+  </si>
+  <si>
+    <t>"112233445566778896.000000"</t>
+  </si>
+  <si>
+    <t>Testing if it can handle edge cases</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1278,6 +1308,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1623,7 +1654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1722,12 +1753,54 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1740,59 +1813,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2085,19 +2119,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="78" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="78" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.88671875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2108,22 +2142,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
@@ -2310,16 +2344,16 @@
       <c r="C10" s="7">
         <v>123456</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="39" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
@@ -2330,10 +2364,10 @@
       <c r="C11" s="5">
         <v>7891011</v>
       </c>
-      <c r="D11" s="55"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="40"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2346,16 +2380,16 @@
       <c r="C12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="39" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
@@ -2366,10 +2400,10 @@
       <c r="C13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="40"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2382,16 +2416,16 @@
       <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="39" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
@@ -2402,10 +2436,10 @@
       <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="40"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
@@ -2418,16 +2452,16 @@
       <c r="C16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="41" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="1"/>
@@ -2438,10 +2472,10 @@
       <c r="C17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="37"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="42"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,14 +2486,14 @@
         <v>73</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="36" t="s">
+      <c r="D18" s="47"/>
+      <c r="E18" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="39" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
@@ -2468,10 +2502,10 @@
       <c r="A19" s="14"/>
       <c r="B19" s="13"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="40"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2484,16 +2518,16 @@
       <c r="C20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="39" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
@@ -2502,10 +2536,10 @@
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="47"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="40"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
@@ -2773,13 +2807,13 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
       <c r="F33" s="26" t="s">
         <v>2</v>
       </c>
@@ -2841,7 +2875,7 @@
       <c r="B36" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="36" t="s">
         <v>89</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -2883,183 +2917,183 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="54" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="7">
         <v>1</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="F38" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="46" t="s">
+      <c r="G38" s="39" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="7">
         <v>3</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="47"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="40"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="54" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="42" t="s">
+      <c r="F40" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="46" t="s">
+      <c r="G40" s="39" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="49"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="47"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="40"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="54" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="48" t="s">
+      <c r="D42" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="36" t="s">
+      <c r="E42" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="42" t="s">
+      <c r="F42" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="36" t="s">
+      <c r="G42" s="41" t="s">
         <v>81</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="37"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="42"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="54" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="42" t="s">
+      <c r="F44" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="36" t="s">
+      <c r="G44" s="41" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="45"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="37"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="42"/>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B46" s="54" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="E46" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="42" t="s">
+      <c r="F46" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="36" t="s">
+      <c r="G46" s="41" t="s">
         <v>84</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="41"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="37"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="42"/>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3109,11 +3143,21 @@
       <c r="B51" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="3"/>
+      <c r="C51" s="7">
+        <v>32</v>
+      </c>
+      <c r="D51" s="7">
+        <v>32</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3123,11 +3167,21 @@
       <c r="B52" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="3"/>
+      <c r="C52" s="7">
+        <v>1234567890</v>
+      </c>
+      <c r="D52" s="7">
+        <v>1234567890</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
@@ -3137,21 +3191,31 @@
       <c r="B53" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="3"/>
+      <c r="C53" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
       <c r="F54" s="26" t="s">
         <v>2</v>
       </c>
@@ -3348,18 +3412,36 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="E38:E39"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A54:E54"/>
@@ -3376,36 +3458,18 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{256EE760-E688-4C56-B416-E0BCCD36032A}"/>

</xml_diff>

<commit_message>
uploading test cases runned and working program
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 2/Final-Project-Test-Cases-version-2.xlsx
+++ b/Documents/Test cases/Version 2/Final-Project-Test-Cases-version-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca cpp\CPR101\group project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680095C8-FF14-4B8A-B372-8E9F7D77326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D019884-56A7-4A5A-BABE-AE99560B95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -515,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{9836CAFB-1676-45A2-B128-23BB665358E1}">
+    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{9836CAFB-1676-45A2-B128-23BB665358E1}">
       <text>
         <r>
           <rPr>
@@ -559,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0" shapeId="0" xr:uid="{76394C31-CC6A-443F-856B-B9E505AC5129}">
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{76394C31-CC6A-443F-856B-B9E505AC5129}">
       <text>
         <r>
           <rPr>
@@ -624,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C55" authorId="0" shapeId="0" xr:uid="{60A2FF5C-FCB2-44D1-9E75-0B74877A989D}">
+    <comment ref="C56" authorId="0" shapeId="0" xr:uid="{60A2FF5C-FCB2-44D1-9E75-0B74877A989D}">
       <text>
         <r>
           <rPr>
@@ -650,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D55" authorId="0" shapeId="0" xr:uid="{BF659CD8-BAF3-4C12-B572-156B71229E3D}">
+    <comment ref="D56" authorId="0" shapeId="0" xr:uid="{BF659CD8-BAF3-4C12-B572-156B71229E3D}">
       <text>
         <r>
           <rPr>
@@ -695,7 +695,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E55" authorId="0" shapeId="0" xr:uid="{C07AA38A-C9DD-4AEA-BCE7-50B9653F9760}">
+    <comment ref="E56" authorId="0" shapeId="0" xr:uid="{C07AA38A-C9DD-4AEA-BCE7-50B9653F9760}">
       <text>
         <r>
           <rPr>
@@ -709,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{6E1CC602-D3D0-4102-916C-BF2983576C05}">
+    <comment ref="F56" authorId="0" shapeId="0" xr:uid="{6E1CC602-D3D0-4102-916C-BF2983576C05}">
       <text>
         <r>
           <rPr>
@@ -732,7 +732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G55" authorId="0" shapeId="0" xr:uid="{C6A33B25-CB18-4D20-9BB9-F794950874F8}">
+    <comment ref="G56" authorId="0" shapeId="0" xr:uid="{C6A33B25-CB18-4D20-9BB9-F794950874F8}">
       <text>
         <r>
           <rPr>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="114">
   <si>
     <t>Comments</t>
   </si>
@@ -1178,6 +1178,41 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>one,two,three,four</t>
+  </si>
+  <si>
+    <t>Several words together,Several words apart,Several words alone are but a work of art</t>
+  </si>
+  <si>
+    <t>"Phrase #1 is 'one'"
+"Phrase #2 is 'two'"
+"Phrase #3 is 'three'"
+"Phrase #4 is 'four'"</t>
+  </si>
+  <si>
+    <t>"Phrase #1 is 'one two three four"</t>
+  </si>
+  <si>
+    <t>"Type a few phrases separated by comma(q - to quit):"</t>
+  </si>
+  <si>
+    <t>"Phrase #1 is 'Several words together"
+"Phrase #2 is 'Several words apart"
+"Phrase #3 is 'Several words alone are but a work of art"</t>
+  </si>
+  <si>
+    <t>All four "phrases" provided have been correctly separated and displayed sequentially with the correct positional identifiers.</t>
+  </si>
+  <si>
+    <t>All four "phrases" provided have been correctly recognized as a single entity and displayed as belonging to one word. This is expected, as the specified delimiter was not used.</t>
+  </si>
+  <si>
+    <t>An empty user-input string has correctly been ignored, as no characters or words exist.</t>
+  </si>
+  <si>
+    <t>Multiple comma delimited phrases have been correctly identified, separated, and displayed with the appropriate positional value.</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1649,12 +1684,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1756,6 +1862,37 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1825,8 +1962,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2117,24 +2254,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="78" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="106" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
@@ -2142,22 +2279,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
@@ -2165,7 +2302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -2189,7 +2326,7 @@
       </c>
       <c r="H3" s="21"/>
     </row>
-    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2350,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -2237,7 +2374,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
@@ -2262,7 +2399,7 @@
       <c r="H6" s="21"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -2286,7 +2423,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
@@ -2310,7 +2447,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>6</v>
       </c>
@@ -2334,7 +2471,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
@@ -2344,33 +2481,33 @@
       <c r="C10" s="7">
         <v>123456</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="50" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5">
         <v>7891011</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="40"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="51"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
@@ -2380,33 +2517,33 @@
       <c r="C12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="50" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="13"/>
       <c r="C13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="40"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="51"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
@@ -2416,33 +2553,33 @@
       <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="50" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="51"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
@@ -2452,33 +2589,33 @@
       <c r="C16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="52" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="13"/>
       <c r="C17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="42"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="53"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -2486,29 +2623,29 @@
         <v>73</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="41" t="s">
+      <c r="D18" s="58"/>
+      <c r="E18" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="50" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="13"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="40"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="51"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
@@ -2518,31 +2655,31 @@
       <c r="C20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="50" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="40"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="51"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
@@ -2566,7 +2703,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="193.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +2727,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2751,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>3</v>
       </c>
@@ -2638,7 +2775,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>3</v>
       </c>
@@ -2662,7 +2799,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +2823,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>3</v>
       </c>
@@ -2710,7 +2847,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>3</v>
       </c>
@@ -2734,7 +2871,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>3</v>
       </c>
@@ -2758,7 +2895,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>3</v>
       </c>
@@ -2782,7 +2919,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>3</v>
       </c>
@@ -2806,14 +2943,14 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
+    <row r="33" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="26" t="s">
         <v>2</v>
       </c>
@@ -2821,7 +2958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>9</v>
       </c>
@@ -2844,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>6</v>
       </c>
@@ -2857,7 +2994,7 @@
       <c r="D35" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="40" t="s">
         <v>33</v>
       </c>
       <c r="F35" s="15" t="s">
@@ -2868,7 +3005,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>6</v>
       </c>
@@ -2881,7 +3018,7 @@
       <c r="D36" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="40" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="15" t="s">
@@ -2892,7 +3029,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>6</v>
       </c>
@@ -2905,7 +3042,7 @@
       <c r="D37" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="40" t="s">
         <v>33</v>
       </c>
       <c r="F37" s="15" t="s">
@@ -2916,358 +3053,395 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52" t="s">
+    <row r="38" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="65" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="7">
         <v>1</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="F38" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="50" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
-      <c r="B39" s="55"/>
+    <row r="39" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="64"/>
+      <c r="B39" s="66"/>
       <c r="C39" s="7">
         <v>3</v>
       </c>
-      <c r="D39" s="57"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="40"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="51"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52" t="s">
+    <row r="40" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="65" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="39" t="s">
+      <c r="G40" s="50" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
-      <c r="B41" s="55"/>
+    <row r="41" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="64"/>
+      <c r="B41" s="66"/>
       <c r="C41" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="57"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="40"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="51"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
+    <row r="42" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="65" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="58" t="s">
+      <c r="D42" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="F42" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="41" t="s">
+      <c r="G42" s="52" t="s">
         <v>81</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
-      <c r="B43" s="55"/>
+    <row r="43" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="64"/>
+      <c r="B43" s="66"/>
       <c r="C43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="57"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="42"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="53"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
+    <row r="44" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="65" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="F44" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="41" t="s">
+      <c r="G44" s="52" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="55"/>
+    <row r="45" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="64"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="59"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="42"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="53"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="52" t="s">
+    <row r="46" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="65" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="41" t="s">
+      <c r="E46" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="41" t="s">
+      <c r="G46" s="52" t="s">
         <v>84</v>
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
-      <c r="B47" s="55"/>
+    <row r="47" spans="1:9" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="64"/>
+      <c r="B47" s="66"/>
       <c r="C47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="59"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="42"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="71"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="46" t="s">
+        <v>110</v>
+      </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C49" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D50" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="7">
-        <v>32</v>
-      </c>
-      <c r="D51" s="7">
-        <v>32</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C51" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="7">
-        <v>1234567890</v>
+        <v>32</v>
       </c>
       <c r="D52" s="7">
-        <v>1234567890</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>97</v>
+        <v>32</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>94</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="G52" s="43" t="s">
+        <v>96</v>
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B53" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1234567890</v>
+      </c>
+      <c r="D53" s="7">
+        <v>1234567890</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="60" t="s">
+      <c r="C54" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="D53" s="60" t="s">
+      <c r="D54" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E54" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G53" s="16" t="s">
+      <c r="G54" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="43" t="s">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="26" t="s">
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G54" s="25" t="s">
+      <c r="G55" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22" t="s">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B56" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C56" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D56" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="24" t="s">
+      <c r="E56" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F56" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G56" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="3"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -3276,12 +3450,12 @@
       <c r="G57" s="3"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -3290,12 +3464,12 @@
       <c r="G58" s="3"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -3304,12 +3478,12 @@
       <c r="G59" s="3"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -3318,12 +3492,12 @@
       <c r="G60" s="3"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -3332,25 +3506,26 @@
       <c r="G61" s="3"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="3"/>
       <c r="F62" s="15"/>
       <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -3358,12 +3533,12 @@
       <c r="F63" s="15"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -3371,12 +3546,12 @@
       <c r="F64" s="15"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -3384,12 +3559,12 @@
       <c r="F65" s="15"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -3397,18 +3572,31 @@
       <c r="F66" s="15"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B67" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="4"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="58">
@@ -3444,7 +3632,7 @@
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A55:E55"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D12:D13"/>
@@ -3486,12 +3674,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="89.5546875" customWidth="1"/>
+    <col min="1" max="1" width="89.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>10</v>
       </c>

</xml_diff>